<commit_message>
Allow lookup of emails from another spreadsheet.
</commit_message>
<xml_diff>
--- a/DECS Excel Add-Ins/test files/email addresses.xlsx
+++ b/DECS Excel Add-Ins/test files/email addresses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\DECS-Office-AddIns\DECS Excel Add-Ins\test files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9248CB08-D037-4016-AD69-2E5A56B08937}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2460E550-3F12-46E5-A126-68D3FE465052}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{527C4681-A4DD-4DC8-BAC5-1E93725C5E5C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>email</t>
   </si>
@@ -55,13 +55,25 @@
   </si>
   <si>
     <t>ryoleary@ucsd.edu</t>
+  </si>
+  <si>
+    <t>q3bui@health.ucsd.edu</t>
+  </si>
+  <si>
+    <t>b1kwan@health.ucsd.edu</t>
+  </si>
+  <si>
+    <t>Alenz@health.ucsd.edu</t>
+  </si>
+  <si>
+    <t>nphreaner@health.ucsd.edu</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -77,16 +89,328 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color indexed="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -94,18 +418,229 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="46">
+    <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="24" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="32" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="36" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="40" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="21" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="25" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="29" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="33" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="37" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="41" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="26" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="30" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="34" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="38" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="42" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="19" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="23" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="27" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="31" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="35" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="39" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="8" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="12" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="14" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="17" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="7" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="3" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="4" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="5" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="6" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink 3" xfId="44" xr:uid="{50E8D27F-4D0C-4158-9C1E-16C420131602}"/>
+    <cellStyle name="Input" xfId="10" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="13" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="9" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 17" xfId="43" xr:uid="{D1CD8368-3414-42C2-BDA2-5338CB2715A8}"/>
+    <cellStyle name="Normal 2" xfId="45" xr:uid="{70645535-F75A-4F65-BC8C-F04D3E6050F7}"/>
+    <cellStyle name="Note" xfId="16" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="11" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="2" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="18" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="15" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -417,66 +952,100 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{336F5226-8F66-4686-A7E7-1CCF19A7ADE4}">
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="A4:XFD4"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.5703125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B2" s="1"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B4" s="1"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B5" s="1"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B7" s="1"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B9" s="1"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="B10" s="1"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="6"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="6"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -489,6 +1058,7 @@
     <hyperlink ref="A2" r:id="rId7" xr:uid="{597599A1-13EA-4284-BB6A-0723DAA4F0F5}"/>
     <hyperlink ref="A3" r:id="rId8" xr:uid="{BD8DD073-5AA7-4979-8FDD-1CB0BF9FA06E}"/>
     <hyperlink ref="A4" r:id="rId9" xr:uid="{A3E4E962-F9C1-44E7-811A-6BCCBB550630}"/>
+    <hyperlink ref="A13" r:id="rId10" xr:uid="{DC309B41-87F7-40FE-B2C1-68F4E066DB4B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>